<commit_message>
introduce Visualization of results
</commit_message>
<xml_diff>
--- a/Results_2B/Results_Alpha025/Results_SegRec/Results_Cross/Results_CSETNet/seed_results_CSETNet_balanced.xlsx
+++ b/Results_2B/Results_Alpha025/Results_SegRec/Results_Cross/Results_CSETNet/seed_results_CSETNet_balanced.xlsx
@@ -498,31 +498,31 @@
         <v>0.74</v>
       </c>
       <c r="C2" t="n">
-        <v>0.73</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8</v>
+        <v>0.76</v>
       </c>
       <c r="E2" t="n">
-        <v>0.96</v>
+        <v>0.91</v>
       </c>
       <c r="F2" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="G2" t="n">
-        <v>0.84</v>
+        <v>0.87</v>
       </c>
       <c r="H2" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="J2" t="n">
-        <v>0.91</v>
+        <v>0.89</v>
       </c>
       <c r="K2" t="n">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="3">
@@ -530,34 +530,34 @@
         <v>71</v>
       </c>
       <c r="B3" t="n">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="C3" t="n">
-        <v>0.68</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D3" t="n">
         <v>0.78</v>
       </c>
       <c r="E3" t="n">
-        <v>0.96</v>
+        <v>0.92</v>
       </c>
       <c r="F3" t="n">
-        <v>0.96</v>
+        <v>0.95</v>
       </c>
       <c r="G3" t="n">
-        <v>0.87</v>
+        <v>0.88</v>
       </c>
       <c r="H3" t="n">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="I3" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J3" t="n">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="K3" t="n">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="4">
@@ -565,34 +565,34 @@
         <v>101</v>
       </c>
       <c r="B4" t="n">
-        <v>0.74</v>
+        <v>0.78</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.73</v>
       </c>
       <c r="D4" t="n">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="E4" t="n">
-        <v>0.96</v>
+        <v>0.8</v>
       </c>
       <c r="F4" t="n">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="G4" t="n">
-        <v>0.86</v>
+        <v>0.92</v>
       </c>
       <c r="H4" t="n">
-        <v>0.92</v>
+        <v>0.9</v>
       </c>
       <c r="I4" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J4" t="n">
-        <v>0.91</v>
+        <v>0.88</v>
       </c>
       <c r="K4" t="n">
-        <v>0.87</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="5">
@@ -600,31 +600,31 @@
         <v>113</v>
       </c>
       <c r="B5" t="n">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
       <c r="C5" t="n">
         <v>0.7</v>
       </c>
       <c r="D5" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.79</v>
       </c>
       <c r="E5" t="n">
-        <v>0.92</v>
+        <v>0.96</v>
       </c>
       <c r="F5" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="G5" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.89</v>
       </c>
-      <c r="H5" t="n">
-        <v>0.92</v>
-      </c>
       <c r="I5" t="n">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="J5" t="n">
-        <v>0.89</v>
+        <v>0.9</v>
       </c>
       <c r="K5" t="n">
         <v>0.87</v>
@@ -635,16 +635,16 @@
         <v>127</v>
       </c>
       <c r="B6" t="n">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="C6" t="n">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
       <c r="D6" t="n">
-        <v>0.78</v>
+        <v>0.73</v>
       </c>
       <c r="E6" t="n">
-        <v>0.78</v>
+        <v>0.96</v>
       </c>
       <c r="F6" t="n">
         <v>0.98</v>
@@ -656,10 +656,10 @@
         <v>0.91</v>
       </c>
       <c r="I6" t="n">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="J6" t="n">
-        <v>0.92</v>
+        <v>0.88</v>
       </c>
       <c r="K6" t="n">
         <v>0.86</v>
@@ -670,34 +670,34 @@
         <v>131</v>
       </c>
       <c r="B7" t="n">
-        <v>0.79</v>
+        <v>0.77</v>
       </c>
       <c r="C7" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.66</v>
       </c>
       <c r="D7" t="n">
-        <v>0.77</v>
+        <v>0.74</v>
       </c>
       <c r="E7" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.93</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="I7" t="n">
         <v>0.96</v>
       </c>
-      <c r="G7" t="n">
+      <c r="J7" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.87</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.88</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.93</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.86</v>
       </c>
     </row>
     <row r="8">
@@ -705,34 +705,34 @@
         <v>139</v>
       </c>
       <c r="B8" t="n">
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
       <c r="C8" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="D8" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="E8" t="n">
-        <v>0.93</v>
+        <v>0.97</v>
       </c>
       <c r="F8" t="n">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="G8" t="n">
         <v>0.88</v>
       </c>
       <c r="H8" t="n">
-        <v>0.89</v>
+        <v>0.93</v>
       </c>
       <c r="I8" t="n">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="J8" t="n">
-        <v>0.89</v>
+        <v>0.88</v>
       </c>
       <c r="K8" t="n">
-        <v>0.86</v>
+        <v>0.87</v>
       </c>
     </row>
     <row r="9">
@@ -740,25 +740,25 @@
         <v>149</v>
       </c>
       <c r="B9" t="n">
-        <v>0.78</v>
+        <v>0.76</v>
       </c>
       <c r="C9" t="n">
         <v>0.74</v>
       </c>
       <c r="D9" t="n">
-        <v>0.79</v>
+        <v>0.72</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.95</v>
       </c>
       <c r="F9" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="G9" t="n">
-        <v>0.89</v>
+        <v>0.91</v>
       </c>
       <c r="H9" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="I9" t="n">
         <v>0.95</v>
@@ -775,31 +775,31 @@
         <v>157</v>
       </c>
       <c r="B10" t="n">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="C10" t="n">
         <v>0.68</v>
       </c>
       <c r="D10" t="n">
-        <v>0.79</v>
+        <v>0.72</v>
       </c>
       <c r="E10" t="n">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="F10" t="n">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="G10" t="n">
-        <v>0.83</v>
+        <v>0.91</v>
       </c>
       <c r="H10" t="n">
         <v>0.91</v>
       </c>
       <c r="I10" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J10" t="n">
-        <v>0.88</v>
+        <v>0.91</v>
       </c>
       <c r="K10" t="n">
         <v>0.85</v>
@@ -810,34 +810,34 @@
         <v>163</v>
       </c>
       <c r="B11" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="C11" t="n">
-        <v>0.74</v>
+        <v>0.73</v>
       </c>
       <c r="D11" t="n">
-        <v>0.77</v>
+        <v>0.8</v>
       </c>
       <c r="E11" t="n">
-        <v>0.95</v>
+        <v>0.88</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.96</v>
       </c>
       <c r="G11" t="n">
-        <v>0.88</v>
+        <v>0.87</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.93</v>
       </c>
       <c r="J11" t="n">
         <v>0.9</v>
       </c>
       <c r="K11" t="n">
-        <v>0.87</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="12">
@@ -845,31 +845,31 @@
         <v>173</v>
       </c>
       <c r="B12" t="n">
-        <v>0.76</v>
+        <v>0.77</v>
       </c>
       <c r="C12" t="n">
-        <v>0.7</v>
+        <v>0.71</v>
       </c>
       <c r="D12" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="E12" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F12" t="n">
         <v>0.98</v>
       </c>
-      <c r="F12" t="n">
-        <v>0.97</v>
-      </c>
       <c r="G12" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="H12" t="n">
-        <v>0.91</v>
+        <v>0.92</v>
       </c>
       <c r="I12" t="n">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="J12" t="n">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="K12" t="n">
         <v>0.87</v>
@@ -880,31 +880,31 @@
         <v>181</v>
       </c>
       <c r="B13" t="n">
-        <v>0.72</v>
+        <v>0.78</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.73</v>
       </c>
       <c r="D13" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.71</v>
       </c>
       <c r="E13" t="n">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="F13" t="n">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="G13" t="n">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="H13" t="n">
-        <v>0.91</v>
+        <v>0.9</v>
       </c>
       <c r="I13" t="n">
-        <v>0.95</v>
+        <v>0.93</v>
       </c>
       <c r="J13" t="n">
-        <v>0.92</v>
+        <v>0.89</v>
       </c>
       <c r="K13" t="n">
         <v>0.87</v>
@@ -918,31 +918,31 @@
         <v>0.72</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="D14" t="n">
-        <v>0.82</v>
+        <v>0.73</v>
       </c>
       <c r="E14" t="n">
-        <v>0.84</v>
+        <v>0.93</v>
       </c>
       <c r="F14" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="G14" t="n">
-        <v>0.87</v>
+        <v>0.91</v>
       </c>
       <c r="H14" t="n">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
       <c r="I14" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J14" t="n">
         <v>0.88</v>
       </c>
       <c r="K14" t="n">
-        <v>0.85</v>
+        <v>0.86</v>
       </c>
     </row>
     <row r="15">
@@ -950,34 +950,34 @@
         <v>521</v>
       </c>
       <c r="B15" t="n">
-        <v>0.77</v>
+        <v>0.72</v>
       </c>
       <c r="C15" t="n">
-        <v>0.71</v>
+        <v>0.68</v>
       </c>
       <c r="D15" t="n">
-        <v>0.78</v>
+        <v>0.75</v>
       </c>
       <c r="E15" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.98</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.89</v>
+      </c>
+      <c r="I15" t="n">
         <v>0.95</v>
       </c>
-      <c r="F15" t="n">
-        <v>0.92</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0.86</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0.9399999999999999</v>
-      </c>
       <c r="J15" t="n">
-        <v>0.88</v>
+        <v>0.89</v>
       </c>
       <c r="K15" t="n">
-        <v>0.86</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="16">
@@ -993,25 +993,25 @@
         <v>0.7</v>
       </c>
       <c r="D16" t="n">
-        <v>0.79</v>
+        <v>0.76</v>
       </c>
       <c r="E16" t="n">
         <v>0.93</v>
       </c>
       <c r="F16" t="n">
-        <v>0.96</v>
+        <v>0.98</v>
       </c>
       <c r="G16" t="n">
-        <v>0.87</v>
+        <v>0.9</v>
       </c>
       <c r="H16" t="n">
         <v>0.91</v>
       </c>
       <c r="I16" t="n">
-        <v>0.95</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="J16" t="n">
-        <v>0.9</v>
+        <v>0.89</v>
       </c>
       <c r="K16" t="n">
         <v>0.86</v>

</xml_diff>